<commit_message>
Add new Ophelia support
</commit_message>
<xml_diff>
--- a/automation_fa/issue_by_amount.xlsx
+++ b/automation_fa/issue_by_amount.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\REL_Automation\automation_fa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REL_Automation\automation_fa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF3FEFEB-1866-4D63-883A-3F8AD34273A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05344F5-8ED9-448B-A030-4000E50FED45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="285" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>amount</t>
   </si>
@@ -32,13 +32,40 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>Erase Fail</t>
+  </si>
+  <si>
+    <t>Prog Fail</t>
+  </si>
+  <si>
+    <t>UECC</t>
+  </si>
+  <si>
+    <t>PS: BBM  EH  EPWR block bad(deVBA)</t>
+  </si>
+  <si>
+    <t>EPWR Failure after recovery  fail (GBB)</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>PS: EH  EF  Recovery(reqId|VBA|msgType|cmd70)</t>
+  </si>
+  <si>
+    <t>PS: EH  PF Recovery(reqID|VBA|msgType Cmd70 blkType|PEC)</t>
+  </si>
+  <si>
+    <t>PS: EH  REH  UNRECOVERABLE(dgId|reqIdx|msgType|EHmap|VBA|savedMap|moreInfo)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,6 +83,18 @@
       <color rgb="FF6AAB73"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,13 +132,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -421,7 +464,9 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="4" t="s">
+        <v>9</v>
+      </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -461,7 +506,52 @@
         <v>500000</v>
       </c>
     </row>
+    <row r="4" spans="1:25" ht="16.5">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" ht="16.5">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" ht="16.5">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" ht="16.5">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>